<commit_message>
OK order book basic
</commit_message>
<xml_diff>
--- a/order_book_fake.xlsx
+++ b/order_book_fake.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/jd2322_ic_ac_uk/Documents/Design Engineering/Design Engineering Year 4/Master's Project/Code/Order Book Auction/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code Master's Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{388D4ABB-6661-4AAD-8067-43C9F5473169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4768548-F00D-427F-B46C-4A0473924C88}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBABA3E-1FCB-4123-A621-1F3BD6388196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{06926657-A2D9-4645-BDB6-A54B3E9AEACE}"/>
   </bookViews>
@@ -422,8 +422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99CD8DE6-5B41-4569-B463-A2A1A39B2479}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="185" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -818,11 +818,10 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
-        <v>7</v>
+        <v>-2</v>
       </c>
       <c r="D10" s="1">
         <v>0.82299999999999995</v>

</xml_diff>